<commit_message>
Update EBase and PBase database structure
</commit_message>
<xml_diff>
--- a/cytation_H1_plate1_GFP.xlsx
+++ b/cytation_H1_plate1_GFP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerald\Desktop\School Stuff\Sem 7\FYP\EBase + PBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D441817E-4AA1-46D9-A6F8-3211E9DD27B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3370E662-9AB1-4891-AFD9-EF088BB9FF39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
   <si>
     <t>Time</t>
   </si>
@@ -322,12 +322,6 @@
     <t>H12</t>
   </si>
   <si>
-    <t>Protocol</t>
-  </si>
-  <si>
-    <t>Experiment identifier</t>
-  </si>
-  <si>
     <t>Type of experiment</t>
   </si>
   <si>
@@ -353,6 +347,18 @@
   </si>
   <si>
     <t>Type2</t>
+  </si>
+  <si>
+    <t>Experiment Identifier</t>
+  </si>
+  <si>
+    <t>Measurement</t>
+  </si>
+  <si>
+    <t>Plasmid name</t>
+  </si>
+  <si>
+    <t>plasmid2</t>
   </si>
 </sst>
 </file>
@@ -728,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB10FFB-459B-41C4-ACB3-FD9998693FA8}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -739,44 +745,50 @@
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>103</v>
+      <c r="G1" s="4" t="s">
+        <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" t="s">
         <v>106</v>
-      </c>
-      <c r="B2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C2" t="s">
-        <v>108</v>
       </c>
       <c r="D2">
         <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F2" t="s">
-        <v>105</v>
+        <v>103</v>
+      </c>
+      <c r="G2" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>